<commit_message>
Estruturação do plano de medição
</commit_message>
<xml_diff>
--- a/documentation/MA/Tamandua_001_05.05.12_Plano de Medição.xlsx
+++ b/documentation/MA/Tamandua_001_05.05.12_Plano de Medição.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="360" windowWidth="18735" windowHeight="11640" firstSheet="1" activeTab="4"/>
@@ -14,7 +14,7 @@
     <sheet name="Banco de Dados de Métricas" sheetId="6" r:id="rId5"/>
     <sheet name="Análise" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="246">
   <si>
     <t>Indicadores</t>
   </si>
@@ -327,9 +327,6 @@
   </si>
   <si>
     <t>GRE</t>
-  </si>
-  <si>
-    <t>GPP</t>
   </si>
   <si>
     <t>GPR</t>
@@ -1513,12 +1510,15 @@
   <si>
     <t>Semana 03</t>
   </si>
+  <si>
+    <t>Semana 04</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1732,7 +1732,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1832,38 +1832,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1884,6 +1854,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1896,12 +1902,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1989,7 +1992,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2024,7 +2026,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -2200,14 +2201,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5:E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.140625" customWidth="1"/>
@@ -2219,207 +2220,206 @@
     <col min="8" max="8" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35"/>
-      <c r="B1" s="35" t="s">
+    <row r="1" spans="1:8" s="7" customFormat="1">
+      <c r="A1" s="44"/>
+      <c r="B1" s="44" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35" t="s">
+      <c r="F1" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="F1" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="G1" s="35" t="s">
+      <c r="H1" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="H1" s="35" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="7" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
+    </row>
+    <row r="2" spans="1:8" s="7" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A2" s="44"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+    </row>
+    <row r="3" spans="1:8" s="7" customFormat="1">
+      <c r="A3" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-    </row>
-    <row r="3" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="B3" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="C3" s="47"/>
+      <c r="D3" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="39" t="s">
+      <c r="E3" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="F3" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="G3" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="F3" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="G3" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="H3" s="37" t="s">
+    </row>
+    <row r="4" spans="1:8" s="7" customFormat="1" ht="45.75" customHeight="1">
+      <c r="A4" s="44"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+    </row>
+    <row r="5" spans="1:8" s="7" customFormat="1">
+      <c r="A5" s="44"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="48" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" s="7" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-    </row>
-    <row r="5" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="39" t="s">
+      <c r="E5" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="E5" s="38" t="s">
+      <c r="F5" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="G5" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" s="46"/>
+    </row>
+    <row r="6" spans="1:8" s="7" customFormat="1">
+      <c r="A6" s="44"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="F5" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="G5" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="H5" s="37"/>
-    </row>
-    <row r="6" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-    </row>
-    <row r="7" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+    </row>
+    <row r="7" spans="1:8" s="7" customFormat="1" ht="45">
+      <c r="A7" s="44"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
       <c r="D7" s="17" t="s">
         <v>59</v>
       </c>
       <c r="E7" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="F7" s="16" t="s">
         <v>115</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>116</v>
       </c>
       <c r="G7" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="H7" s="37"/>
-    </row>
-    <row r="8" spans="1:8" s="7" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35" t="s">
-        <v>117</v>
-      </c>
-      <c r="B8" s="38" t="s">
-        <v>120</v>
-      </c>
-      <c r="C8" s="38"/>
+      <c r="H7" s="46"/>
+    </row>
+    <row r="8" spans="1:8" s="7" customFormat="1" ht="32.25" customHeight="1">
+      <c r="A8" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="47" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="47"/>
       <c r="D8" s="13" t="s">
         <v>57</v>
       </c>
       <c r="E8" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="G8" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8" s="45" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="7" customFormat="1" ht="32.25" customHeight="1">
+      <c r="A9" s="44"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="F8" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="G8" s="36" t="s">
-        <v>71</v>
-      </c>
-      <c r="H8" s="36" t="s">
+      <c r="F9" s="15" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" s="7" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="13" t="s">
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+    </row>
+    <row r="10" spans="1:8" s="7" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A10" s="44"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E10" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="F9" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-    </row>
-    <row r="10" spans="1:8" s="7" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="E10" s="14" t="s">
+      <c r="F10" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+    </row>
+    <row r="11" spans="1:8" s="7" customFormat="1" ht="45">
+      <c r="A11" s="44"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="E11" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="F10" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-    </row>
-    <row r="11" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="35"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>124</v>
-      </c>
       <c r="F11" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
+        <v>129</v>
+      </c>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="H1:H2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="H8:H11"/>
     <mergeCell ref="H3:H7"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="B8:C11"/>
     <mergeCell ref="G8:G11"/>
-    <mergeCell ref="G1:G2"/>
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="B3:C7"/>
     <mergeCell ref="D3:D4"/>
@@ -2428,7 +2428,8 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="G5:G6"/>
-    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:D2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2436,14 +2437,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="B22" sqref="B22:C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11" style="5" customWidth="1"/>
     <col min="2" max="2" width="40.7109375" bestFit="1" customWidth="1"/>
@@ -2454,7 +2455,7 @@
     <col min="7" max="7" width="20.7109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="18" t="s">
         <v>64</v>
       </c>
@@ -2474,148 +2475,148 @@
         <v>6</v>
       </c>
       <c r="G1" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="33" customHeight="1">
+      <c r="A2" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>79</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F2" s="19" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30">
+      <c r="A3" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>81</v>
-      </c>
       <c r="C3" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D3" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>195</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>196</v>
       </c>
       <c r="F3" s="19" t="s">
         <v>13</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30">
       <c r="A4" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F4" s="19" t="s">
         <v>13</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="45">
       <c r="A5" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B5" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>85</v>
-      </c>
       <c r="E5" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F5" s="19" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30">
       <c r="A6" s="19" t="s">
         <v>62</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="45">
+      <c r="A7" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" s="20" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>88</v>
-      </c>
       <c r="C7" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F7" s="19" t="s">
         <v>13</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30">
       <c r="A8" s="19" t="s">
         <v>62</v>
       </c>
@@ -2623,329 +2624,329 @@
         <v>67</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F8" s="19" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="45">
       <c r="A9" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F9" s="19" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="60">
       <c r="A10" s="19" t="s">
         <v>62</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F10" s="19" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="45">
       <c r="A11" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F11" s="19" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30">
       <c r="A12" s="19" t="s">
         <v>62</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F12" s="19" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30">
       <c r="A13" s="19" t="s">
         <v>62</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F13" s="19" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="45.75" customHeight="1">
       <c r="A14" s="19" t="s">
         <v>62</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D14" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="E14" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="E14" s="15" t="s">
-        <v>201</v>
-      </c>
       <c r="F14" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="33" customHeight="1">
       <c r="A15" s="21" t="s">
         <v>62</v>
       </c>
       <c r="B15" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="D15" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="C15" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="D15" s="22" t="s">
+      <c r="E15" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="E15" s="15" t="s">
-        <v>204</v>
-      </c>
       <c r="F15" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="45">
       <c r="A16" s="21" t="s">
         <v>62</v>
       </c>
       <c r="B16" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D16" s="22" t="s">
         <v>205</v>
       </c>
-      <c r="C16" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="D16" s="22" t="s">
+      <c r="E16" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="E16" s="15" t="s">
-        <v>207</v>
-      </c>
       <c r="F16" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="45">
       <c r="A17" s="19" t="s">
         <v>62</v>
       </c>
       <c r="B17" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="D17" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="C17" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="D17" s="15" t="s">
+      <c r="E17" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="60">
+      <c r="A18" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="C18" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="F17" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="G17" s="15" t="s">
+      <c r="F18" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="G18" s="15" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="G18" s="15" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="45">
       <c r="A19" s="19" t="s">
         <v>62</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C19" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="G19" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="D19" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:7" s="12" customFormat="1" ht="30">
       <c r="A20" s="24" t="s">
         <v>62</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C20" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="D20" s="23" t="s">
         <v>226</v>
       </c>
-      <c r="D20" s="23" t="s">
+      <c r="E20" s="23" t="s">
         <v>227</v>
       </c>
-      <c r="E20" s="23" t="s">
-        <v>228</v>
-      </c>
       <c r="F20" s="24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G20" s="23" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="60">
       <c r="A21" s="19" t="s">
         <v>62</v>
       </c>
       <c r="B21" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="G21" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C21" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="D21" s="15" t="s">
+    </row>
+    <row r="22" spans="1:7" ht="45">
+      <c r="A22" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B22" s="15" t="s">
         <v>209</v>
       </c>
-      <c r="E21" s="15" t="s">
-        <v>182</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="B22" s="15" t="s">
+      <c r="C22" s="15" t="s">
         <v>210</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>211</v>
       </c>
       <c r="D22" s="16" t="s">
         <v>22</v>
@@ -2957,18 +2958,18 @@
         <v>13</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="60">
       <c r="A23" s="24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B23" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="C23" s="15" t="s">
         <v>212</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>213</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>26</v>
@@ -2980,18 +2981,18 @@
         <v>13</v>
       </c>
       <c r="G23" s="21" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="90">
       <c r="A24" s="23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>61</v>
@@ -3003,18 +3004,18 @@
         <v>13</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="75">
       <c r="A25" s="23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>31</v>
@@ -3026,7 +3027,7 @@
         <v>13</v>
       </c>
       <c r="G25" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -3037,14 +3038,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" customWidth="1"/>
@@ -3058,7 +3059,7 @@
     <col min="10" max="10" width="51.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="7" customFormat="1" ht="30">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -3084,10 +3085,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="7" customFormat="1" ht="105">
       <c r="A2" s="15" t="s">
         <v>8</v>
       </c>
@@ -3095,7 +3096,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>11</v>
@@ -3104,7 +3105,7 @@
         <v>12</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G2" s="16" t="s">
         <v>13</v>
@@ -3113,11 +3114,11 @@
         <v>14</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J2" s="25"/>
     </row>
-    <row r="3" spans="1:10" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="7" customFormat="1" ht="105">
       <c r="A3" s="15" t="s">
         <v>15</v>
       </c>
@@ -3125,7 +3126,7 @@
         <v>16</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>18</v>
@@ -3134,7 +3135,7 @@
         <v>19</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G3" s="16" t="s">
         <v>13</v>
@@ -3143,10 +3144,10 @@
         <v>20</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" s="7" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="7" customFormat="1" ht="90">
       <c r="A4" s="15" t="s">
         <v>21</v>
       </c>
@@ -3154,7 +3155,7 @@
         <v>34</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>60</v>
@@ -3163,7 +3164,7 @@
         <v>35</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G4" s="15" t="s">
         <v>13</v>
@@ -3172,10 +3173,10 @@
         <v>24</v>
       </c>
       <c r="I4" s="19" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="7" customFormat="1" ht="105">
       <c r="A5" s="15" t="s">
         <v>25</v>
       </c>
@@ -3183,7 +3184,7 @@
         <v>37</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>38</v>
@@ -3192,7 +3193,7 @@
         <v>39</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G5" s="15" t="s">
         <v>13</v>
@@ -3201,27 +3202,27 @@
         <v>24</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="7" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="7" customFormat="1" ht="90">
       <c r="A6" s="15" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>40</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F6" s="26" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G6" s="15" t="s">
         <v>13</v>
@@ -3230,25 +3231,25 @@
         <v>24</v>
       </c>
       <c r="I6" s="19" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="7" customFormat="1" ht="105">
       <c r="A7" s="27" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="27" t="s">
+        <v>219</v>
+      </c>
+      <c r="C7" s="27" t="s">
         <v>220</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="D7" s="28" t="s">
         <v>221</v>
-      </c>
-      <c r="D7" s="28" t="s">
-        <v>222</v>
       </c>
       <c r="E7" s="27"/>
       <c r="F7" s="27" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G7" s="27" t="s">
         <v>13</v>
@@ -3256,15 +3257,15 @@
       <c r="H7" s="27"/>
       <c r="I7" s="29"/>
     </row>
-    <row r="8" spans="1:10" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="7" customFormat="1" ht="105">
       <c r="A8" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B8" s="23" t="s">
+        <v>223</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>224</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>225</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>41</v>
@@ -3273,7 +3274,7 @@
         <v>42</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G8" s="16" t="s">
         <v>13</v>
@@ -3285,7 +3286,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="7" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="7" customFormat="1" ht="165">
       <c r="A9" s="15" t="s">
         <v>36</v>
       </c>
@@ -3293,7 +3294,7 @@
         <v>45</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>46</v>
@@ -3302,7 +3303,7 @@
         <v>47</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G9" s="16" t="s">
         <v>13</v>
@@ -3314,7 +3315,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="7" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="7" customFormat="1" ht="120">
       <c r="A10" s="15" t="s">
         <v>44</v>
       </c>
@@ -3322,7 +3323,7 @@
         <v>50</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>51</v>
@@ -3331,19 +3332,19 @@
         <v>52</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="7" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="7" customFormat="1" ht="120">
       <c r="A11" s="15" t="s">
         <v>48</v>
       </c>
@@ -3351,7 +3352,7 @@
         <v>54</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>55</v>
@@ -3360,19 +3361,19 @@
         <v>56</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G11" s="15" t="s">
         <v>13</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="7" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="7" customFormat="1" ht="120">
       <c r="A12" s="15" t="s">
         <v>53</v>
       </c>
@@ -3380,16 +3381,16 @@
         <v>58</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G12" s="15" t="s">
         <v>13</v>
@@ -3401,13 +3402,13 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="3"/>
       <c r="E13" s="2"/>
       <c r="G13" s="8"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="3"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -3422,19 +3423,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B22" sqref="B16:B22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="39.85546875" style="11" customWidth="1"/>
     <col min="3" max="3" width="45.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1">
       <c r="A1" s="31" t="s">
         <v>63</v>
       </c>
@@ -3445,323 +3448,260 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+    <row r="2" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A2" s="53" t="s">
         <v>66</v>
       </c>
       <c r="B2" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="50" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A3" s="53"/>
+      <c r="B3" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="43" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="44"/>
-      <c r="B3" s="21" t="s">
+      <c r="C3" s="50"/>
+    </row>
+    <row r="4" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A4" s="53"/>
+      <c r="B4" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="43"/>
-    </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
-      <c r="B4" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="51" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="44"/>
+    <row r="5" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A5" s="53"/>
       <c r="B5" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="41"/>
-    </row>
-    <row r="6" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
+      <c r="C5" s="51"/>
+    </row>
+    <row r="6" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A6" s="53"/>
       <c r="B6" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="52" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A7" s="53"/>
+      <c r="B7" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="42" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
-      <c r="B7" s="21" t="s">
+      <c r="C7" s="52"/>
+    </row>
+    <row r="8" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A8" s="53"/>
+      <c r="B8" s="21" t="s">
         <v>76</v>
-      </c>
-      <c r="C7" s="42"/>
-    </row>
-    <row r="8" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
-      <c r="B8" s="21" t="s">
-        <v>77</v>
       </c>
       <c r="C8" s="32" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="44" t="s">
+    <row r="9" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A9" s="53" t="s">
         <v>68</v>
       </c>
       <c r="B9" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A10" s="53"/>
+      <c r="B10" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="43" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
-      <c r="B10" s="21" t="s">
+      <c r="C10" s="50"/>
+    </row>
+    <row r="11" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A11" s="53"/>
+      <c r="B11" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="43"/>
-    </row>
-    <row r="11" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
-      <c r="B11" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="C11" s="41" t="s">
+      <c r="C11" s="51" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
+    <row r="12" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A12" s="53"/>
       <c r="B12" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="41"/>
-    </row>
-    <row r="13" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
+      <c r="C12" s="51"/>
+    </row>
+    <row r="13" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A13" s="53"/>
       <c r="B13" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="52" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A14" s="53"/>
+      <c r="B14" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="42" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="44"/>
-      <c r="B14" s="21" t="s">
+      <c r="C14" s="52"/>
+    </row>
+    <row r="15" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A15" s="53"/>
+      <c r="B15" s="21" t="s">
         <v>76</v>
-      </c>
-      <c r="C14" s="42"/>
-    </row>
-    <row r="15" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
-      <c r="B15" s="21" t="s">
-        <v>77</v>
       </c>
       <c r="C15" s="32" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="44" t="s">
+    <row r="16" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A16" s="53" t="s">
         <v>69</v>
       </c>
       <c r="B16" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="50" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A17" s="53"/>
+      <c r="B17" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="43" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="44"/>
-      <c r="B17" s="21" t="s">
+      <c r="C17" s="50"/>
+    </row>
+    <row r="18" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A18" s="53"/>
+      <c r="B18" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="43"/>
-    </row>
-    <row r="18" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
-      <c r="B18" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="C18" s="41" t="s">
+      <c r="C18" s="51" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+    <row r="19" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A19" s="53"/>
       <c r="B19" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="41"/>
-    </row>
-    <row r="20" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
+      <c r="C19" s="51"/>
+    </row>
+    <row r="20" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A20" s="53"/>
       <c r="B20" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="52" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A21" s="53"/>
+      <c r="B21" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="42" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="44"/>
-      <c r="B21" s="21" t="s">
+      <c r="C21" s="52"/>
+    </row>
+    <row r="22" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A22" s="53"/>
+      <c r="B22" s="21" t="s">
         <v>76</v>
-      </c>
-      <c r="C21" s="42"/>
-    </row>
-    <row r="22" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
-      <c r="B22" s="21" t="s">
-        <v>77</v>
       </c>
       <c r="C22" s="32" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="44" t="s">
+    <row r="23" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A23" s="53" t="s">
         <v>70</v>
       </c>
       <c r="B23" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="50" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A24" s="53"/>
+      <c r="B24" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="43" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
-      <c r="B24" s="21" t="s">
+      <c r="C24" s="50"/>
+    </row>
+    <row r="25" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A25" s="53"/>
+      <c r="B25" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="C24" s="43"/>
-    </row>
-    <row r="25" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
-      <c r="B25" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" s="41" t="s">
+      <c r="C25" s="51" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="44"/>
+    <row r="26" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A26" s="53"/>
       <c r="B26" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="41"/>
-    </row>
-    <row r="27" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="44"/>
+      <c r="C26" s="51"/>
+    </row>
+    <row r="27" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A27" s="53"/>
       <c r="B27" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="52" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A28" s="53"/>
+      <c r="B28" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="42" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
-      <c r="B28" s="21" t="s">
+      <c r="C28" s="52"/>
+    </row>
+    <row r="29" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1">
+      <c r="A29" s="53"/>
+      <c r="B29" s="21" t="s">
         <v>76</v>
-      </c>
-      <c r="C28" s="42"/>
-    </row>
-    <row r="29" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
-      <c r="B29" s="21" t="s">
-        <v>77</v>
       </c>
       <c r="C29" s="32" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="44" t="s">
-        <v>71</v>
-      </c>
-      <c r="B30" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="C30" s="43" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="44"/>
-      <c r="B31" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="C31" s="43"/>
-    </row>
-    <row r="32" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="44"/>
-      <c r="B32" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="C32" s="41" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="44"/>
-      <c r="B33" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="C33" s="41"/>
-    </row>
-    <row r="34" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="44"/>
-      <c r="B34" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="C34" s="42" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="44"/>
-      <c r="B35" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="C35" s="42"/>
-    </row>
-    <row r="36" spans="1:3" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="44"/>
-      <c r="B36" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="C36" s="32" t="s">
-        <v>49</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="16">
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="A9:A15"/>
     <mergeCell ref="A16:A22"/>
     <mergeCell ref="A23:A29"/>
-    <mergeCell ref="A30:A36"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C27:C28"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="C34:C35"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" location="Indicadores!A3" display="Indicador da estimativa de esforço"/>
@@ -3780,10 +3720,6 @@
     <hyperlink ref="C25" location="Indicadores!A4" display="Índice de desempenho de custos acumulado - CPI"/>
     <hyperlink ref="C27:C28" location="Indicadores!A9" display="Indicador de laudos de avaliação realizadas pela garantia de qualidade"/>
     <hyperlink ref="C29" location="Indicadores!A10" display="Indicador de não conformidades"/>
-    <hyperlink ref="C30" location="Indicadores!A3" display="Indicador da estimativa de esforço"/>
-    <hyperlink ref="C32" location="Indicadores!A4" display="Índice de desempenho de custos acumulado - CPI"/>
-    <hyperlink ref="C34:C35" location="Indicadores!A9" display="Indicador de laudos de avaliação realizadas pela garantia de qualidade"/>
-    <hyperlink ref="C36" location="Indicadores!A10" display="Indicador de não conformidades"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3791,446 +3727,537 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.5703125" customWidth="1"/>
     <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+    <col min="4" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
-        <v>230</v>
-      </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
+      <c r="A2" s="54" t="s">
+        <v>229</v>
+      </c>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="34"/>
       <c r="B3" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C3" s="34" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="34">
         <v>1</v>
       </c>
-      <c r="B4" s="47" t="s">
-        <v>81</v>
+      <c r="B4" s="37" t="s">
+        <v>80</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>232</v>
-      </c>
-      <c r="E4" s="46"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+      <c r="E4" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="34">
         <v>2</v>
       </c>
-      <c r="B5" s="47" t="s">
-        <v>82</v>
+      <c r="B5" s="37" t="s">
+        <v>81</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>231</v>
-      </c>
-      <c r="E5" s="46"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+      <c r="E5" s="36"/>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="34">
         <v>3</v>
       </c>
-      <c r="B6" s="47" t="s">
-        <v>84</v>
+      <c r="B6" s="37" t="s">
+        <v>83</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>231</v>
-      </c>
-      <c r="E6" s="46"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+      <c r="E6" s="36"/>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="34">
         <v>4</v>
       </c>
-      <c r="B7" s="47" t="s">
-        <v>90</v>
+      <c r="B7" s="37" t="s">
+        <v>89</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>231</v>
-      </c>
-      <c r="E7" s="46"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+      <c r="E7" s="36"/>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="34">
         <v>5</v>
       </c>
-      <c r="B8" s="47" t="s">
-        <v>91</v>
+      <c r="B8" s="37" t="s">
+        <v>90</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>231</v>
-      </c>
-      <c r="E8" s="46"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+      <c r="E8" s="36"/>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="34">
         <v>6</v>
       </c>
-      <c r="B9" s="48" t="s">
-        <v>92</v>
+      <c r="B9" s="38" t="s">
+        <v>91</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D9" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="E9" s="36">
+        <v>230.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="42">
+        <v>7</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="D10" s="39" t="s">
         <v>231</v>
       </c>
-      <c r="E9" s="46"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="52">
-        <v>7</v>
-      </c>
-      <c r="B10" s="50" t="s">
-        <v>97</v>
-      </c>
-      <c r="C10" s="51" t="s">
-        <v>143</v>
-      </c>
-      <c r="D10" s="49" t="s">
-        <v>232</v>
-      </c>
-      <c r="E10" s="46"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E10" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="19">
         <v>8</v>
       </c>
       <c r="B11" s="23" t="s">
+        <v>235</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="E11" s="36">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="55" t="s">
         <v>236</v>
       </c>
-      <c r="C11" s="24" t="s">
-        <v>226</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>231</v>
-      </c>
-      <c r="E11" s="46"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="53" t="s">
-        <v>237</v>
-      </c>
-      <c r="B13" s="54"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="55"/>
-    </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="56"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="57"/>
+    </row>
+    <row r="14" spans="1:6" ht="30">
       <c r="A14" s="34"/>
       <c r="B14" s="19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C14" s="34" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="33" t="s">
+        <v>237</v>
+      </c>
+      <c r="E14" s="33" t="s">
         <v>238</v>
       </c>
-      <c r="E14" s="33" t="s">
+      <c r="F14" s="33" t="s">
         <v>239</v>
       </c>
-      <c r="F14" s="33" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="34">
         <v>1</v>
       </c>
-      <c r="B15" s="57" t="s">
-        <v>94</v>
+      <c r="B15" s="43" t="s">
+        <v>93</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="34">
         <v>2</v>
       </c>
-      <c r="B16" s="48" t="s">
-        <v>202</v>
+      <c r="B16" s="38" t="s">
+        <v>201</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>153</v>
-      </c>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="34">
         <v>3</v>
       </c>
-      <c r="B17" s="48" t="s">
-        <v>205</v>
+      <c r="B17" s="38" t="s">
+        <v>204</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>152</v>
-      </c>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="34">
         <v>4</v>
       </c>
-      <c r="B18" s="48" t="s">
-        <v>95</v>
+      <c r="B18" s="38" t="s">
+        <v>94</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="34">
         <v>5</v>
       </c>
-      <c r="B19" s="48" t="s">
-        <v>97</v>
+      <c r="B19" s="38" t="s">
+        <v>96</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="34">
         <v>6</v>
       </c>
-      <c r="B20" s="57" t="s">
-        <v>241</v>
+      <c r="B20" s="43" t="s">
+        <v>240</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="19">
         <v>7</v>
       </c>
-      <c r="B21" s="47" t="s">
-        <v>100</v>
+      <c r="B21" s="37" t="s">
+        <v>99</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="D21" s="46"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="56" t="s">
-        <v>242</v>
-      </c>
-      <c r="B23" s="56"/>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="56"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="58" t="s">
+        <v>241</v>
+      </c>
+      <c r="B23" s="58"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="58"/>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="34"/>
       <c r="B24" s="20" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C24" s="19" t="s">
         <v>2</v>
       </c>
       <c r="D24" s="34" t="s">
+        <v>242</v>
+      </c>
+      <c r="E24" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="E24" s="34" t="s">
+      <c r="F24" s="34" t="s">
         <v>244</v>
       </c>
-      <c r="F24" s="34" t="s">
+      <c r="G24" s="35" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" s="34">
         <v>1</v>
       </c>
-      <c r="B25" s="47" t="s">
-        <v>86</v>
+      <c r="B25" s="37" t="s">
+        <v>85</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="D25" s="34">
+        <v>0</v>
+      </c>
+      <c r="E25" s="34">
+        <v>0</v>
+      </c>
+      <c r="F25" s="34">
+        <v>0</v>
+      </c>
+      <c r="G25" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="34">
         <v>2</v>
       </c>
-      <c r="B26" s="47" t="s">
-        <v>88</v>
+      <c r="B26" s="37" t="s">
+        <v>87</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="D26" s="34">
+        <v>0</v>
+      </c>
+      <c r="E26" s="34">
+        <v>0</v>
+      </c>
+      <c r="F26" s="34">
+        <v>0</v>
+      </c>
+      <c r="G26" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="34">
         <v>3</v>
       </c>
-      <c r="B27" s="47" t="s">
+      <c r="B27" s="37" t="s">
         <v>67</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="D27" s="34">
+        <v>0</v>
+      </c>
+      <c r="E27" s="34">
+        <v>0</v>
+      </c>
+      <c r="F27" s="34">
+        <v>0</v>
+      </c>
+      <c r="G27" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="34">
         <v>4</v>
       </c>
-      <c r="B28" s="47" t="s">
-        <v>89</v>
+      <c r="B28" s="37" t="s">
+        <v>88</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="D28" s="34">
+        <v>0</v>
+      </c>
+      <c r="E28" s="34">
+        <v>0</v>
+      </c>
+      <c r="F28" s="34">
+        <v>0</v>
+      </c>
+      <c r="G28" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="34">
         <v>5</v>
       </c>
-      <c r="B29" s="47" t="s">
-        <v>93</v>
+      <c r="B29" s="37" t="s">
+        <v>92</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
-    </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="D29" s="34">
+        <v>0</v>
+      </c>
+      <c r="E29" s="34">
+        <v>0</v>
+      </c>
+      <c r="F29" s="34">
+        <v>0</v>
+      </c>
+      <c r="G29" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="30">
       <c r="A30" s="34">
         <v>6</v>
       </c>
-      <c r="B30" s="57" t="s">
+      <c r="B30" s="43" t="s">
+        <v>209</v>
+      </c>
+      <c r="C30" s="33" t="s">
         <v>210</v>
       </c>
-      <c r="C30" s="33" t="s">
-        <v>211</v>
-      </c>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D30" s="34">
+        <v>0</v>
+      </c>
+      <c r="E30" s="34">
+        <v>0</v>
+      </c>
+      <c r="F30" s="34">
+        <v>0</v>
+      </c>
+      <c r="G30" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="34">
         <v>7</v>
       </c>
-      <c r="B31" s="57" t="s">
+      <c r="B31" s="43" t="s">
+        <v>211</v>
+      </c>
+      <c r="C31" s="33" t="s">
         <v>212</v>
       </c>
-      <c r="C31" s="33" t="s">
-        <v>213</v>
-      </c>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="34"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D31" s="34">
+        <v>0</v>
+      </c>
+      <c r="E31" s="34">
+        <v>0</v>
+      </c>
+      <c r="F31" s="34">
+        <v>0</v>
+      </c>
+      <c r="G31" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" s="34">
         <v>8</v>
       </c>
-      <c r="B32" s="57" t="s">
-        <v>214</v>
+      <c r="B32" s="43" t="s">
+        <v>213</v>
       </c>
       <c r="C32" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="D32" s="34">
+        <v>0</v>
+      </c>
+      <c r="E32" s="34">
+        <v>0</v>
+      </c>
+      <c r="F32" s="34">
+        <v>0</v>
+      </c>
+      <c r="G32" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="34">
         <v>9</v>
       </c>
-      <c r="B33" s="57" t="s">
-        <v>215</v>
+      <c r="B33" s="43" t="s">
+        <v>214</v>
       </c>
       <c r="C33" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
+        <v>126</v>
+      </c>
+      <c r="D33" s="34">
+        <v>0</v>
+      </c>
+      <c r="E33" s="34">
+        <v>0</v>
+      </c>
+      <c r="F33" s="34">
+        <v>0</v>
+      </c>
+      <c r="G33" s="35">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4243,12 +4270,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>